<commit_message>
Commit setelah technical meet dengan mas ganal
</commit_message>
<xml_diff>
--- a/ExtractionResultExcel/ExtractionResults11062024.xlsx
+++ b/ExtractionResultExcel/ExtractionResults11062024.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ProjectUiPath\ICSTAR\EmployeeDataChangeVerification\ExtractionResultExcel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Bootcamp\ICStar Hackathon\Neo Team 1\ExtractionResultExcel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FE48626-37C6-4EF2-9F0A-FACDB8D35AA1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DA21E5C-1BD5-41E4-9401-E32BF9DBFA8B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1464" yWindow="1464" windowWidth="17280" windowHeight="8880" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="7005" yWindow="3645" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="KTP" sheetId="2" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="35">
   <si>
     <t>NIK</t>
   </si>
@@ -470,13 +470,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:R4"/>
+  <dimension ref="A1:R2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -532,7 +532,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:18" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>18</v>
       </c>
@@ -585,118 +585,6 @@
         <v>18</v>
       </c>
       <c r="R2" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B3" t="s">
-        <v>19</v>
-      </c>
-      <c r="C3" t="s">
-        <v>20</v>
-      </c>
-      <c r="D3" t="s">
-        <v>21</v>
-      </c>
-      <c r="E3" t="s">
-        <v>22</v>
-      </c>
-      <c r="F3" t="s">
-        <v>23</v>
-      </c>
-      <c r="G3" t="s">
-        <v>24</v>
-      </c>
-      <c r="H3" t="s">
-        <v>25</v>
-      </c>
-      <c r="I3" t="s">
-        <v>26</v>
-      </c>
-      <c r="J3" t="s">
-        <v>27</v>
-      </c>
-      <c r="K3" t="s">
-        <v>28</v>
-      </c>
-      <c r="L3" t="s">
-        <v>29</v>
-      </c>
-      <c r="M3" t="s">
-        <v>30</v>
-      </c>
-      <c r="N3" t="s">
-        <v>31</v>
-      </c>
-      <c r="O3" t="s">
-        <v>32</v>
-      </c>
-      <c r="P3" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>18</v>
-      </c>
-      <c r="R3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>18</v>
-      </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>20</v>
-      </c>
-      <c r="D4" t="s">
-        <v>21</v>
-      </c>
-      <c r="E4" t="s">
-        <v>22</v>
-      </c>
-      <c r="F4" t="s">
-        <v>23</v>
-      </c>
-      <c r="G4" t="s">
-        <v>24</v>
-      </c>
-      <c r="H4" t="s">
-        <v>25</v>
-      </c>
-      <c r="I4" t="s">
-        <v>26</v>
-      </c>
-      <c r="J4" t="s">
-        <v>27</v>
-      </c>
-      <c r="K4" t="s">
-        <v>28</v>
-      </c>
-      <c r="L4" t="s">
-        <v>29</v>
-      </c>
-      <c r="M4" t="s">
-        <v>30</v>
-      </c>
-      <c r="N4" t="s">
-        <v>31</v>
-      </c>
-      <c r="O4" t="s">
-        <v>32</v>
-      </c>
-      <c r="P4" t="s">
-        <v>33</v>
-      </c>
-      <c r="Q4" t="s">
-        <v>18</v>
-      </c>
-      <c r="R4" s="1" t="s">
         <v>34</v>
       </c>
     </row>

</xml_diff>